<commit_message>
Struccter fixed, Docs Started, No URBS
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GES2SF\everything\Diploma\Diploma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\source\Diploma_git\Diploma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E985329A-3E3E-4C36-A2E5-72C4F50CFD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B59411-22CB-406A-9198-B780F1F78915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="14660" windowWidth="19420" windowHeight="11500" xr2:uid="{99BC40B1-1046-4B75-B04D-28D3C539FC4D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{99BC40B1-1046-4B75-B04D-28D3C539FC4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Компоненти</t>
   </si>
@@ -53,12 +51,6 @@
     <t>Магазин</t>
   </si>
   <si>
-    <t>Farnell</t>
-  </si>
-  <si>
-    <t>Comet Electronics</t>
-  </si>
-  <si>
     <t>MCP6291T-E/OT</t>
   </si>
   <si>
@@ -71,13 +63,35 @@
     <t>Operational Amplifier, Single, 1 Channels, 10 MHz, 7 V/µs, 2.4V to 6V, SOT-23, 5 Pins</t>
   </si>
   <si>
-    <t>Arduino Nano 33 IoT(no headers)</t>
-  </si>
-  <si>
     <t>OSTB8BS4C2B LED</t>
   </si>
   <si>
     <t xml:space="preserve">5.0x5.0x1.5mm, </t>
+  </si>
+  <si>
+    <t>Raspberry Pi Pico</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Pico 2 is a low-cost, high-performance microcontroller board with flexible digital interfaces. Key features include:
+RP2350 
+Dual Cortex-M33 up to 150MHz
+520KB of SRAM, 4MB flash memory
+USB 1.1 with device and host support
+Low-power sleep and dormant modes
+Drag-and-drop programming using mass storage over USB
+26× GPIO pins, 3 ADC
+2× SPI, 2× I2C, 2× UART, 3× 12-bit 500ksps Analogue to Digital Converter (ADC), 24× controllable PWM channels
+2× Timer with 4 alarms, 1× AON Timer
+Temperature sensor</t>
+  </si>
+  <si>
+    <t>SMD Resistors/Capacitors 1206</t>
+  </si>
+  <si>
+    <t>2n3904 Transistor</t>
+  </si>
+  <si>
+    <t>Shcottkey Diods</t>
   </si>
 </sst>
 </file>
@@ -134,16 +148,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -459,96 +483,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28589AB2-C83C-4EE1-B9C0-44ACA9F244B4}">
-  <dimension ref="B1:D9"/>
+  <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
-    <col min="3" max="3" width="72" customWidth="1"/>
-    <col min="4" max="4" width="25.08984375" customWidth="1"/>
+    <col min="1" max="1" width="9.06640625" style="2"/>
+    <col min="2" max="2" width="33.265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.06640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.265625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="2:6" ht="199.5" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B9:D9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{089A42FD-8798-4842-B148-B1A212D80247}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D527A8E8-0B49-47B8-A74C-D767962EC92C}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{C7AA132C-582C-4E49-949D-AE4F4B3958FB}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{621B25B8-ADE8-4780-A093-F7E8181AF0EB}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{688FC4A8-5193-4B02-A775-42968BE897D2}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{089A42FD-8798-4842-B148-B1A212D80247}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{D527A8E8-0B49-47B8-A74C-D767962EC92C}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{C7AA132C-582C-4E49-949D-AE4F4B3958FB}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{688FC4A8-5193-4B02-A775-42968BE897D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>